<commit_message>
Add | Adding OpenStack Dataset
</commit_message>
<xml_diff>
--- a/result/score.xlsx
+++ b/result/score.xlsx
@@ -463,26 +463,26 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[[30331  2576]
- [  993   313]]</t>
+          <t>[[30288  2619]
+ [  909   397]]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[[30564  2343]
- [  752   554]]</t>
+          <t>[[30328  2579]
+ [  878   428]]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[[29507  3400]
- [  742   564]]</t>
+          <t>[[30548  2359]
+ [  958   348]]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[[30375  2532]
- [  669   637]]</t>
+          <t>[[30334  2573]
+ [  720   586]]</t>
         </is>
       </c>
     </row>
@@ -493,16 +493,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8956829275421624</v>
+        <v>0.8968813024289013</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9095373103790957</v>
+        <v>0.8989565369888639</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8789349077835911</v>
+        <v>0.9030485487972408</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9064390728670388</v>
+        <v>0.9037500365358198</v>
       </c>
     </row>
     <row r="4">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1492252681764005</v>
+        <v>0.1837112447940768</v>
       </c>
       <c r="C4" t="n">
-        <v>0.263621222935998</v>
+        <v>0.1984697426385347</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2140417457305503</v>
+        <v>0.1734363319212559</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2846927374301676</v>
+        <v>0.2624860022396416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add | BGL Dataset
</commit_message>
<xml_diff>
--- a/result/score.xlsx
+++ b/result/score.xlsx
@@ -463,26 +463,26 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[[30288  2619]
- [  909   397]]</t>
+          <t>[[96503  4301]
+ [ 2516    53]]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[[30328  2579]
- [  878   428]]</t>
+          <t>[[98920  1884]
+ [ 2529    40]]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[[30548  2359]
- [  958   348]]</t>
+          <t>[[100403    401]
+ [   560   2009]]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[[30334  2573]
- [  720   586]]</t>
+          <t>[[95738  5066]
+ [  560  2009]]</t>
         </is>
       </c>
     </row>
@@ -493,16 +493,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8968813024289013</v>
+        <v>0.9340543468797462</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8989565369888639</v>
+        <v>0.9573099358633299</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9030485487972408</v>
+        <v>0.9907035686301066</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9037500365358198</v>
+        <v>0.9455757306066381</v>
       </c>
     </row>
     <row r="4">
@@ -512,16 +512,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1837112447940768</v>
+        <v>0.01531128123645818</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1984697426385347</v>
+        <v>0.01780547518361896</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1734363319212559</v>
+        <v>0.8069893552922273</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2624860022396416</v>
+        <v>0.4166321028618831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Excel file by condition
</commit_message>
<xml_diff>
--- a/result/score.xlsx
+++ b/result/score.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,38 +474,38 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[[12262    77]
- [  303   250]]</t>
+          <t>[[12242    97]
+ [  243   310]]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[[12275    64]
- [  303   250]]</t>
+          <t>[[12292    47]
+ [  319   234]]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[[12283    56]
- [  315   238]]</t>
+          <t>[[12285    54]
+ [  321   232]]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[[12250    89]
- [  247   306]]</t>
+          <t>[[12162   177]
+ [  280   273]]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[[12246    93]
- [  427   126]]</t>
+          <t>[[12302    37]
+ [  425   128]]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[[12293    46]
- [  319   234]]</t>
+          <t>[[12300    39]
+ [  381   172]]</t>
         </is>
       </c>
     </row>
@@ -516,22 +516,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9705243561898852</v>
+        <v>0.9736270555383183</v>
       </c>
       <c r="C3" t="n">
-        <v>0.971532733478126</v>
+        <v>0.9716103009618368</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9712224635432827</v>
+        <v>0.9709121936084394</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9739373254731617</v>
+        <v>0.9645516599441514</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9596649084703692</v>
+        <v>0.9641638225255973</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9716878684455477</v>
+        <v>0.9674216568414521</v>
       </c>
     </row>
     <row r="4">
@@ -541,22 +541,47 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5681818181818181</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5767012687427913</v>
+        <v>0.5611510791366906</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5619834710743802</v>
+        <v>0.5530393325387366</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6455696202531646</v>
+        <v>0.5443668993020938</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3264248704663212</v>
+        <v>0.3565459610027855</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5618247298919568</v>
+        <v>0.450261780104712</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7.668647050857544</v>
+      </c>
+      <c r="C5" t="n">
+        <v>18.13580298423767</v>
+      </c>
+      <c r="D5" t="n">
+        <v>15.49525141716003</v>
+      </c>
+      <c r="E5" t="n">
+        <v>7.885470628738403</v>
+      </c>
+      <c r="F5" t="n">
+        <v>57.8807532787323</v>
+      </c>
+      <c r="G5" t="n">
+        <v>71.08479619026184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>